<commit_message>
updated data dictionaries #112
</commit_message>
<xml_diff>
--- a/backend/oeps/data/dictionaries/C_Dict.xlsx
+++ b/backend/oeps/data/dictionaries/C_Dict.xlsx
@@ -1237,18 +1237,10 @@
         </is>
       </c>
       <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr">
@@ -1258,17 +1250,17 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>Ovr65P</t>
+          <t>Age18_64</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>% Population: Age 65+</t>
+          <t>Population: Age 18-64</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>Percentage of population over 65</t>
+          <t>Total adult population under age 65</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
@@ -1288,12 +1280,12 @@
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>15.77</t>
+          <t>1139347</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr">
@@ -1309,43 +1301,63 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>FemP</t>
+          <t>Age0_4</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>% Population that is Female</t>
-        </is>
-      </c>
-      <c r="V9" t="inlineStr"/>
+          <t>Population: Age 0-4</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>Total population between age 0-4</t>
+        </is>
+      </c>
       <c r="W9" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -1353,25 +1365,29 @@
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t xml:space="preserve">ACS </t>
+          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>American Community Survey (5-Year Estimate)</t>
+          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
         </is>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>60.0</t>
-        </is>
-      </c>
-      <c r="AC9" t="inlineStr"/>
+          <t>79897</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
+        </is>
+      </c>
       <c r="AD9" t="inlineStr"/>
     </row>
     <row r="10">
@@ -1380,43 +1396,63 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>MaleP</t>
+          <t>Age5_14</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>% Population that is Male</t>
-        </is>
-      </c>
-      <c r="V10" t="inlineStr"/>
+          <t>Population: Age 5-14</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>Total population between age 5-14</t>
+        </is>
+      </c>
       <c r="W10" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -1424,25 +1460,29 @@
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t xml:space="preserve">ACS </t>
+          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
         </is>
       </c>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>American Community Survey (5-Year Estimate)</t>
+          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
         </is>
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>60.0</t>
-        </is>
-      </c>
-      <c r="AC10" t="inlineStr"/>
+          <t>122034</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
+        </is>
+      </c>
       <c r="AD10" t="inlineStr"/>
     </row>
     <row r="11">
@@ -1451,43 +1491,63 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>MedAge</t>
+          <t>Age15_19</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>Median age</t>
-        </is>
-      </c>
-      <c r="V11" t="inlineStr"/>
+          <t>Population: Age 15-19</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>Total population between age 15-19</t>
+        </is>
+      </c>
       <c r="W11" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -1495,25 +1555,29 @@
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t xml:space="preserve">ACS </t>
+          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>American Community Survey (5-Year Estimate)</t>
+          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
         </is>
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>60.0</t>
-        </is>
-      </c>
-      <c r="AC11" t="inlineStr"/>
+          <t>68706</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
+        </is>
+      </c>
       <c r="AD11" t="inlineStr"/>
     </row>
     <row r="12">
@@ -1522,43 +1586,63 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>Ovr16P</t>
+          <t>Age20_24</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>% Population over 16 years</t>
-        </is>
-      </c>
-      <c r="V12" t="inlineStr"/>
+          <t>Population: Age 20-24</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>Total population between age 20-24</t>
+        </is>
+      </c>
       <c r="W12" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -1566,25 +1650,29 @@
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t xml:space="preserve">ACS </t>
+          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>American Community Survey (5-Year Estimate)</t>
+          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
         </is>
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>60.0</t>
-        </is>
-      </c>
-      <c r="AC12" t="inlineStr"/>
+          <t>114772</t>
+        </is>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
+        </is>
+      </c>
       <c r="AD12" t="inlineStr"/>
     </row>
     <row r="13">
@@ -1593,43 +1681,63 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>Ovr18P</t>
+          <t>Age15_44</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>% Population over 18 years</t>
-        </is>
-      </c>
-      <c r="V13" t="inlineStr"/>
+          <t>Population: Age 15-44</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>Total population between age 15-44</t>
+        </is>
+      </c>
       <c r="W13" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -1637,25 +1745,29 @@
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t xml:space="preserve">ACS </t>
+          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
         </is>
       </c>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>American Community Survey (5-Year Estimate)</t>
+          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
         </is>
       </c>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>60.0</t>
-        </is>
-      </c>
-      <c r="AC13" t="inlineStr"/>
+          <t>784568</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
+        </is>
+      </c>
       <c r="AD13" t="inlineStr"/>
     </row>
     <row r="14">
@@ -1664,7 +1776,11 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
@@ -1675,32 +1791,28 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr">
         <is>
-          <t>Ovr21P</t>
+          <t>Age45_54</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>% Population over 21 years</t>
-        </is>
-      </c>
-      <c r="V14" t="inlineStr"/>
+          <t>Population: Age 45-54</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>Total population between age 45-54</t>
+        </is>
+      </c>
       <c r="W14" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -1708,26 +1820,34 @@
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t xml:space="preserve">ACS </t>
+          <t>IPUMS NHGIS</t>
         </is>
       </c>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>American Community Survey (5-Year Estimate)</t>
+          <t>Integrated Public Use Microdata Series National Historic Geographic Information System</t>
         </is>
       </c>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>60.0</t>
-        </is>
-      </c>
-      <c r="AC14" t="inlineStr"/>
-      <c r="AD14" t="inlineStr"/>
+          <t>105</t>
+        </is>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>Data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function, with county subdivisions as the underlying population weights.</t>
+        </is>
+      </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>The 1980 Census data does not allow for disaggregation into Age45_49 and Age50_54 variables, so this variable is used instead. The data itself is from its respective decennial census as downloaded from IPUMS NHGIS and crosswalked to 2010 census tracts using Longitudinal Tract Database crosswalk files. For more on the crosswalk files, see https://s4.ad.brown.edu/Projects/Diversity/researcher/bridging.htm</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1735,43 +1855,63 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>Ovr62P</t>
+          <t>Age55_59</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>% Population over 62 years</t>
-        </is>
-      </c>
-      <c r="V15" t="inlineStr"/>
+          <t>Population: Age 55-59</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>Total population between age 55-59</t>
+        </is>
+      </c>
       <c r="W15" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -1779,25 +1919,29 @@
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t xml:space="preserve">ACS </t>
+          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
         </is>
       </c>
       <c r="Y15" t="inlineStr">
         <is>
-          <t>American Community Survey (5-Year Estimate)</t>
+          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
         </is>
       </c>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="AB15" t="inlineStr">
         <is>
-          <t>60.0</t>
-        </is>
-      </c>
-      <c r="AC15" t="inlineStr"/>
+          <t>94082</t>
+        </is>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
+        </is>
+      </c>
       <c r="AD15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -1806,43 +1950,63 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>SRatio</t>
+          <t>Age60_64</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>Sex ratio for the total population (males per 100 females)</t>
-        </is>
-      </c>
-      <c r="V16" t="inlineStr"/>
+          <t>Population: Age 60-64</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>Total population between age 60-64</t>
+        </is>
+      </c>
       <c r="W16" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -1850,25 +2014,29 @@
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t xml:space="preserve">ACS </t>
+          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>American Community Survey (5-Year Estimate)</t>
+          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
         </is>
       </c>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>60.0</t>
-        </is>
-      </c>
-      <c r="AC16" t="inlineStr"/>
+          <t>90711</t>
+        </is>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
+        </is>
+      </c>
       <c r="AD16" t="inlineStr"/>
     </row>
     <row r="17">
@@ -1877,43 +2045,63 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>SRatio18</t>
+          <t>AgeOv65</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>Sex ratio among adults aged 18 and older (males per 100 females)</t>
-        </is>
-      </c>
-      <c r="V17" t="inlineStr"/>
+          <t>Population: Age 65+</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>Total population at or over age 65</t>
+        </is>
+      </c>
       <c r="W17" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -1921,25 +2109,29 @@
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t xml:space="preserve">ACS </t>
+          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>American Community Survey (5-Year Estimate)</t>
+          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
         </is>
       </c>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>60.0</t>
-        </is>
-      </c>
-      <c r="AC17" t="inlineStr"/>
+          <t>257362</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
+        </is>
+      </c>
       <c r="AD17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -1948,43 +2140,63 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr"/>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>SRatio65</t>
+          <t>Age15_24P</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>Sex ratio among seniors aged 65 and older (males per 100 females)</t>
-        </is>
-      </c>
-      <c r="V18" t="inlineStr"/>
+          <t>% Population: Age 15-24</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>Percentage of population between ages of 15 &amp; 24</t>
+        </is>
+      </c>
       <c r="W18" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -1992,12 +2204,12 @@
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t xml:space="preserve">ACS </t>
+          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
         <is>
-          <t>American Community Survey (5-Year Estimate)</t>
+          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
         </is>
       </c>
       <c r="AA18" t="inlineStr">
@@ -2007,10 +2219,14 @@
       </c>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>60.0</t>
-        </is>
-      </c>
-      <c r="AC18" t="inlineStr"/>
+          <t>11.24</t>
+        </is>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
+        </is>
+      </c>
       <c r="AD18" t="inlineStr"/>
     </row>
     <row r="19">
@@ -2019,43 +2235,63 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
       <c r="R19" t="inlineStr"/>
-      <c r="S19" t="inlineStr"/>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>Und18P</t>
+          <t>Und45P</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>% Population under 18 years old</t>
-        </is>
-      </c>
-      <c r="V19" t="inlineStr"/>
+          <t>% Population: Age under 45</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	Percentage of population below 45 years of age</t>
+        </is>
+      </c>
       <c r="W19" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -2063,12 +2299,12 @@
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t xml:space="preserve">ACS </t>
+          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
         </is>
       </c>
       <c r="Y19" t="inlineStr">
         <is>
-          <t>American Community Survey (5-Year Estimate)</t>
+          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
         </is>
       </c>
       <c r="AA19" t="inlineStr">
@@ -2078,10 +2314,14 @@
       </c>
       <c r="AB19" t="inlineStr">
         <is>
-          <t>60.0</t>
-        </is>
-      </c>
-      <c r="AC19" t="inlineStr"/>
+          <t>60.43</t>
+        </is>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
+        </is>
+      </c>
       <c r="AD19" t="inlineStr"/>
     </row>
     <row r="20">
@@ -2090,16 +2330,36 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr">
         <is>
@@ -2115,18 +2375,26 @@
       </c>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="inlineStr"/>
-      <c r="S20" t="inlineStr"/>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>Und5P</t>
+          <t>Ovr65P</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t xml:space="preserve">% Population under 5 years old </t>
-        </is>
-      </c>
-      <c r="V20" t="inlineStr"/>
+          <t>% Population: Age 65+</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>Percentage of population over 65</t>
+        </is>
+      </c>
       <c r="W20" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -2134,12 +2402,12 @@
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t xml:space="preserve">ACS </t>
+          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
         </is>
       </c>
       <c r="Y20" t="inlineStr">
         <is>
-          <t>American Community Survey (5-Year Estimate)</t>
+          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
         </is>
       </c>
       <c r="AA20" t="inlineStr">
@@ -2149,10 +2417,14 @@
       </c>
       <c r="AB20" t="inlineStr">
         <is>
-          <t>60.0</t>
-        </is>
-      </c>
-      <c r="AC20" t="inlineStr"/>
+          <t>15.77</t>
+        </is>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
+        </is>
+      </c>
       <c r="AD20" t="inlineStr"/>
     </row>
     <row r="21">
@@ -2205,17 +2477,17 @@
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>Age18_64</t>
+          <t>ChildrenP</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>Population: Age 18-64</t>
+          <t>Children %</t>
         </is>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>Total adult population under age 65</t>
+          <t>Percentage of population under age 18</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
@@ -2235,12 +2507,12 @@
       </c>
       <c r="AA21" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>number</t>
         </is>
       </c>
       <c r="AB21" t="inlineStr">
         <is>
-          <t>1139347</t>
+          <t>0.14</t>
         </is>
       </c>
       <c r="AC21" t="inlineStr">
@@ -2256,11 +2528,7 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
           <t>x</t>
@@ -2293,24 +2561,20 @@
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr"/>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr">
         <is>
-          <t>Age0_4</t>
+          <t>Age45_49</t>
         </is>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>Population: Age 0-4</t>
+          <t>Population: Age 45-49</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>Total population between age 0-4</t>
+          <t>Total population between age 45-49</t>
         </is>
       </c>
       <c r="W22" t="inlineStr">
@@ -2320,12 +2584,12 @@
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
+          <t>ACS 2018, 5-Year; 2010 Decennial Census; IPUMS NHGIS</t>
         </is>
       </c>
       <c r="Y22" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
+          <t>American Community Survey 2014-2018 5 Year Estimates; 2010 Decennial Census; Integrated Public Use Microdata Service National Historic Geographic Information Systems</t>
         </is>
       </c>
       <c r="AA22" t="inlineStr">
@@ -2335,15 +2599,15 @@
       </c>
       <c r="AB22" t="inlineStr">
         <is>
-          <t>79897</t>
-        </is>
-      </c>
-      <c r="AC22" t="inlineStr">
-        <is>
-          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
-        </is>
-      </c>
-      <c r="AD22" t="inlineStr"/>
+          <t>467768</t>
+        </is>
+      </c>
+      <c r="AC22" t="inlineStr"/>
+      <c r="AD22" t="inlineStr">
+        <is>
+          <t>1990 and 2000 data from respective decennial censuses downloaded from IPUMS NHGIS and aggregated upwards.</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2351,11 +2615,7 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
           <t>x</t>
@@ -2388,24 +2648,20 @@
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
       <c r="R23" t="inlineStr"/>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr">
         <is>
-          <t>Age5_14</t>
+          <t>Age50_54</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>Population: Age 5-14</t>
+          <t>Population: Age 50-54</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>Total population between age 5-14</t>
+          <t>Total population between age 50-54</t>
         </is>
       </c>
       <c r="W23" t="inlineStr">
@@ -2415,30 +2671,30 @@
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
+          <t>ACS 2018, 5-Year; 2010 Decennial Census; IPUMS NHGIS</t>
         </is>
       </c>
       <c r="Y23" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
+          <t>American Community Survey 2014-2018 5 Year Estimates; 2010 Decennial Census; Integrated Public Use Microdata Service National Historic Geographic Information Systems</t>
         </is>
       </c>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>number</t>
         </is>
       </c>
       <c r="AB23" t="inlineStr">
         <is>
-          <t>122034</t>
-        </is>
-      </c>
-      <c r="AC23" t="inlineStr">
-        <is>
-          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
-        </is>
-      </c>
-      <c r="AD23" t="inlineStr"/>
+          <t>476486</t>
+        </is>
+      </c>
+      <c r="AC23" t="inlineStr"/>
+      <c r="AD23" t="inlineStr">
+        <is>
+          <t>1990 and 2000 data from respective decennial censuses downloaded from IPUMS NHGIS and aggregated upwards.</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2446,21 +2702,9 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
           <t>x</t>
@@ -2483,24 +2727,20 @@
       <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr">
         <is>
-          <t>Age15_19</t>
+          <t>AgeOv18</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>Population: Age 15-19</t>
+          <t>Population: Age 18+</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>Total population between age 15-19</t>
+          <t>Total population at or over age 18</t>
         </is>
       </c>
       <c r="W24" t="inlineStr">
@@ -2510,29 +2750,25 @@
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
+          <t>ACS 2018, 5-Year; 2010 Decennial Census</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
+          <t>American Community Survey 2014-2018 5 Year Estimates; 2010 Decennial Census</t>
         </is>
       </c>
       <c r="AA24" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>number</t>
         </is>
       </c>
       <c r="AB24" t="inlineStr">
         <is>
-          <t>68706</t>
-        </is>
-      </c>
-      <c r="AC24" t="inlineStr">
-        <is>
-          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
-        </is>
-      </c>
+          <t>5661461</t>
+        </is>
+      </c>
+      <c r="AC24" t="inlineStr"/>
       <c r="AD24" t="inlineStr"/>
     </row>
     <row r="25">
@@ -2541,63 +2777,43 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr"/>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr"/>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr">
         <is>
-          <t>Age20_24</t>
+          <t>FemP</t>
         </is>
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>Population: Age 20-24</t>
-        </is>
-      </c>
-      <c r="V25" t="inlineStr">
-        <is>
-          <t>Total population between age 20-24</t>
-        </is>
-      </c>
+          <t>% Population that is Female</t>
+        </is>
+      </c>
+      <c r="V25" t="inlineStr"/>
       <c r="W25" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -2605,29 +2821,25 @@
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
+          <t xml:space="preserve">ACS </t>
         </is>
       </c>
       <c r="Y25" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
+          <t>American Community Survey (5-Year Estimate)</t>
         </is>
       </c>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>number</t>
         </is>
       </c>
       <c r="AB25" t="inlineStr">
         <is>
-          <t>114772</t>
-        </is>
-      </c>
-      <c r="AC25" t="inlineStr">
-        <is>
-          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
-        </is>
-      </c>
+          <t>60.0</t>
+        </is>
+      </c>
+      <c r="AC25" t="inlineStr"/>
       <c r="AD25" t="inlineStr"/>
     </row>
     <row r="26">
@@ -2636,63 +2848,43 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
-      <c r="M26" t="inlineStr"/>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
-      <c r="P26" t="inlineStr"/>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q26" t="inlineStr"/>
       <c r="R26" t="inlineStr"/>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr">
         <is>
-          <t>Age15_44</t>
+          <t>MaleP</t>
         </is>
       </c>
       <c r="U26" t="inlineStr">
         <is>
-          <t>Population: Age 15-44</t>
-        </is>
-      </c>
-      <c r="V26" t="inlineStr">
-        <is>
-          <t>Total population between age 15-44</t>
-        </is>
-      </c>
+          <t>% Population that is Male</t>
+        </is>
+      </c>
+      <c r="V26" t="inlineStr"/>
       <c r="W26" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -2700,29 +2892,25 @@
       </c>
       <c r="X26" t="inlineStr">
         <is>
-          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
+          <t xml:space="preserve">ACS </t>
         </is>
       </c>
       <c r="Y26" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
+          <t>American Community Survey (5-Year Estimate)</t>
         </is>
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>number</t>
         </is>
       </c>
       <c r="AB26" t="inlineStr">
         <is>
-          <t>784568</t>
-        </is>
-      </c>
-      <c r="AC26" t="inlineStr">
-        <is>
-          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
-        </is>
-      </c>
+          <t>60.0</t>
+        </is>
+      </c>
+      <c r="AC26" t="inlineStr"/>
       <c r="AD26" t="inlineStr"/>
     </row>
     <row r="27">
@@ -2731,11 +2919,7 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
@@ -2746,28 +2930,32 @@
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
-      <c r="M27" t="inlineStr"/>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr"/>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q27" t="inlineStr"/>
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr">
         <is>
-          <t>Age45_54</t>
+          <t>MedAge</t>
         </is>
       </c>
       <c r="U27" t="inlineStr">
         <is>
-          <t>Population: Age 45-54</t>
-        </is>
-      </c>
-      <c r="V27" t="inlineStr">
-        <is>
-          <t>Total population between age 45-54</t>
-        </is>
-      </c>
+          <t>Median age</t>
+        </is>
+      </c>
+      <c r="V27" t="inlineStr"/>
       <c r="W27" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -2775,34 +2963,26 @@
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>IPUMS NHGIS</t>
+          <t xml:space="preserve">ACS </t>
         </is>
       </c>
       <c r="Y27" t="inlineStr">
         <is>
-          <t>Integrated Public Use Microdata Series National Historic Geographic Information System</t>
+          <t>American Community Survey (5-Year Estimate)</t>
         </is>
       </c>
       <c r="AA27" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>number</t>
         </is>
       </c>
       <c r="AB27" t="inlineStr">
         <is>
-          <t>105</t>
-        </is>
-      </c>
-      <c r="AC27" t="inlineStr">
-        <is>
-          <t>Data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function, with county subdivisions as the underlying population weights.</t>
-        </is>
-      </c>
-      <c r="AD27" t="inlineStr">
-        <is>
-          <t>The 1980 Census data does not allow for disaggregation into Age45_49 and Age50_54 variables, so this variable is used instead. The data itself is from its respective decennial census as downloaded from IPUMS NHGIS and crosswalked to 2010 census tracts using Longitudinal Tract Database crosswalk files. For more on the crosswalk files, see https://s4.ad.brown.edu/Projects/Diversity/researcher/bridging.htm</t>
-        </is>
-      </c>
+          <t>60.0</t>
+        </is>
+      </c>
+      <c r="AC27" t="inlineStr"/>
+      <c r="AD27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2810,63 +2990,43 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr"/>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr"/>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q28" t="inlineStr"/>
       <c r="R28" t="inlineStr"/>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr">
         <is>
-          <t>Age55_59</t>
+          <t>Ovr16P</t>
         </is>
       </c>
       <c r="U28" t="inlineStr">
         <is>
-          <t>Population: Age 55-59</t>
-        </is>
-      </c>
-      <c r="V28" t="inlineStr">
-        <is>
-          <t>Total population between age 55-59</t>
-        </is>
-      </c>
+          <t>% Population over 16 years</t>
+        </is>
+      </c>
+      <c r="V28" t="inlineStr"/>
       <c r="W28" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -2874,29 +3034,25 @@
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
+          <t xml:space="preserve">ACS </t>
         </is>
       </c>
       <c r="Y28" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
+          <t>American Community Survey (5-Year Estimate)</t>
         </is>
       </c>
       <c r="AA28" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>number</t>
         </is>
       </c>
       <c r="AB28" t="inlineStr">
         <is>
-          <t>94082</t>
-        </is>
-      </c>
-      <c r="AC28" t="inlineStr">
-        <is>
-          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
-        </is>
-      </c>
+          <t>60.0</t>
+        </is>
+      </c>
+      <c r="AC28" t="inlineStr"/>
       <c r="AD28" t="inlineStr"/>
     </row>
     <row r="29">
@@ -2905,63 +3061,43 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
-      <c r="M29" t="inlineStr"/>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr"/>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="inlineStr"/>
-      <c r="S29" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr">
         <is>
-          <t>Age60_64</t>
+          <t>Ovr18P</t>
         </is>
       </c>
       <c r="U29" t="inlineStr">
         <is>
-          <t>Population: Age 60-64</t>
-        </is>
-      </c>
-      <c r="V29" t="inlineStr">
-        <is>
-          <t>Total population between age 60-64</t>
-        </is>
-      </c>
+          <t>% Population over 18 years</t>
+        </is>
+      </c>
+      <c r="V29" t="inlineStr"/>
       <c r="W29" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -2969,29 +3105,25 @@
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
+          <t xml:space="preserve">ACS </t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
+          <t>American Community Survey (5-Year Estimate)</t>
         </is>
       </c>
       <c r="AA29" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>number</t>
         </is>
       </c>
       <c r="AB29" t="inlineStr">
         <is>
-          <t>90711</t>
-        </is>
-      </c>
-      <c r="AC29" t="inlineStr">
-        <is>
-          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
-        </is>
-      </c>
+          <t>60.0</t>
+        </is>
+      </c>
+      <c r="AC29" t="inlineStr"/>
       <c r="AD29" t="inlineStr"/>
     </row>
     <row r="30">
@@ -3000,63 +3132,43 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr"/>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="inlineStr"/>
-      <c r="P30" t="inlineStr"/>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q30" t="inlineStr"/>
       <c r="R30" t="inlineStr"/>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S30" t="inlineStr"/>
       <c r="T30" t="inlineStr">
         <is>
-          <t>AgeOv65</t>
+          <t>Ovr21P</t>
         </is>
       </c>
       <c r="U30" t="inlineStr">
         <is>
-          <t>Population: Age 65+</t>
-        </is>
-      </c>
-      <c r="V30" t="inlineStr">
-        <is>
-          <t>Total population at or over age 65</t>
-        </is>
-      </c>
+          <t>% Population over 21 years</t>
+        </is>
+      </c>
+      <c r="V30" t="inlineStr"/>
       <c r="W30" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -3064,29 +3176,25 @@
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
+          <t xml:space="preserve">ACS </t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
+          <t>American Community Survey (5-Year Estimate)</t>
         </is>
       </c>
       <c r="AA30" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>number</t>
         </is>
       </c>
       <c r="AB30" t="inlineStr">
         <is>
-          <t>257362</t>
-        </is>
-      </c>
-      <c r="AC30" t="inlineStr">
-        <is>
-          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
-        </is>
-      </c>
+          <t>60.0</t>
+        </is>
+      </c>
+      <c r="AC30" t="inlineStr"/>
       <c r="AD30" t="inlineStr"/>
     </row>
     <row r="31">
@@ -3095,63 +3203,43 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr"/>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K31" t="inlineStr"/>
       <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr"/>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="inlineStr"/>
-      <c r="P31" t="inlineStr"/>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr"/>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr">
         <is>
-          <t>Age15_24P</t>
+          <t>Ovr62P</t>
         </is>
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>% Population: Age 15-24</t>
-        </is>
-      </c>
-      <c r="V31" t="inlineStr">
-        <is>
-          <t>Percentage of population between ages of 15 &amp; 24</t>
-        </is>
-      </c>
+          <t>% Population over 62 years</t>
+        </is>
+      </c>
+      <c r="V31" t="inlineStr"/>
       <c r="W31" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -3159,12 +3247,12 @@
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
+          <t xml:space="preserve">ACS </t>
         </is>
       </c>
       <c r="Y31" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
+          <t>American Community Survey (5-Year Estimate)</t>
         </is>
       </c>
       <c r="AA31" t="inlineStr">
@@ -3174,14 +3262,10 @@
       </c>
       <c r="AB31" t="inlineStr">
         <is>
-          <t>11.24</t>
-        </is>
-      </c>
-      <c r="AC31" t="inlineStr">
-        <is>
-          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
-        </is>
-      </c>
+          <t>60.0</t>
+        </is>
+      </c>
+      <c r="AC31" t="inlineStr"/>
       <c r="AD31" t="inlineStr"/>
     </row>
     <row r="32">
@@ -3190,63 +3274,43 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr"/>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr"/>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr"/>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="inlineStr"/>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S32" t="inlineStr"/>
       <c r="T32" t="inlineStr">
         <is>
-          <t>Und45P</t>
+          <t>SRatio</t>
         </is>
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>% Population: Age under 45</t>
-        </is>
-      </c>
-      <c r="V32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">	Percentage of population below 45 years of age</t>
-        </is>
-      </c>
+          <t>Sex ratio for the total population (males per 100 females)</t>
+        </is>
+      </c>
+      <c r="V32" t="inlineStr"/>
       <c r="W32" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -3254,12 +3318,12 @@
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
+          <t xml:space="preserve">ACS </t>
         </is>
       </c>
       <c r="Y32" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
+          <t>American Community Survey (5-Year Estimate)</t>
         </is>
       </c>
       <c r="AA32" t="inlineStr">
@@ -3269,14 +3333,10 @@
       </c>
       <c r="AB32" t="inlineStr">
         <is>
-          <t>60.43</t>
-        </is>
-      </c>
-      <c r="AC32" t="inlineStr">
-        <is>
-          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
-        </is>
-      </c>
+          <t>60.0</t>
+        </is>
+      </c>
+      <c r="AC32" t="inlineStr"/>
       <c r="AD32" t="inlineStr"/>
     </row>
     <row r="33">
@@ -3285,63 +3345,43 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr"/>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr"/>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr"/>
-      <c r="S33" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S33" t="inlineStr"/>
       <c r="T33" t="inlineStr">
         <is>
-          <t>ChildrenP</t>
+          <t>SRatio18</t>
         </is>
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>Children %</t>
-        </is>
-      </c>
-      <c r="V33" t="inlineStr">
-        <is>
-          <t>Percentage of population under age 18</t>
-        </is>
-      </c>
+          <t>Sex ratio among adults aged 18 and older (males per 100 females)</t>
+        </is>
+      </c>
+      <c r="V33" t="inlineStr"/>
       <c r="W33" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -3349,12 +3389,12 @@
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
+          <t xml:space="preserve">ACS </t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
+          <t>American Community Survey (5-Year Estimate)</t>
         </is>
       </c>
       <c r="AA33" t="inlineStr">
@@ -3364,14 +3404,10 @@
       </c>
       <c r="AB33" t="inlineStr">
         <is>
-          <t>0.14</t>
-        </is>
-      </c>
-      <c r="AC33" t="inlineStr">
-        <is>
-          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
-        </is>
-      </c>
+          <t>60.0</t>
+        </is>
+      </c>
+      <c r="AC33" t="inlineStr"/>
       <c r="AD33" t="inlineStr"/>
     </row>
     <row r="34">
@@ -3381,54 +3417,42 @@
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr"/>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
-      <c r="M34" t="inlineStr"/>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr"/>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr"/>
       <c r="T34" t="inlineStr">
         <is>
-          <t>Age45_49</t>
+          <t>SRatio65</t>
         </is>
       </c>
       <c r="U34" t="inlineStr">
         <is>
-          <t>Population: Age 45-49</t>
-        </is>
-      </c>
-      <c r="V34" t="inlineStr">
-        <is>
-          <t>Total population between age 45-49</t>
-        </is>
-      </c>
+          <t>Sex ratio among seniors aged 65 and older (males per 100 females)</t>
+        </is>
+      </c>
+      <c r="V34" t="inlineStr"/>
       <c r="W34" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -3436,30 +3460,26 @@
       </c>
       <c r="X34" t="inlineStr">
         <is>
-          <t>ACS 2018, 5-Year; 2010 Decennial Census; IPUMS NHGIS</t>
+          <t xml:space="preserve">ACS </t>
         </is>
       </c>
       <c r="Y34" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 5 Year Estimates; 2010 Decennial Census; Integrated Public Use Microdata Service National Historic Geographic Information Systems</t>
+          <t>American Community Survey (5-Year Estimate)</t>
         </is>
       </c>
       <c r="AA34" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>number</t>
         </is>
       </c>
       <c r="AB34" t="inlineStr">
         <is>
-          <t>467768</t>
+          <t>60.0</t>
         </is>
       </c>
       <c r="AC34" t="inlineStr"/>
-      <c r="AD34" t="inlineStr">
-        <is>
-          <t>1990 and 2000 data from respective decennial censuses downloaded from IPUMS NHGIS and aggregated upwards.</t>
-        </is>
-      </c>
+      <c r="AD34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3468,54 +3488,42 @@
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr"/>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr"/>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="inlineStr"/>
-      <c r="P35" t="inlineStr"/>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr"/>
       <c r="T35" t="inlineStr">
         <is>
-          <t>Age50_54</t>
+          <t>Und18P</t>
         </is>
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>Population: Age 50-54</t>
-        </is>
-      </c>
-      <c r="V35" t="inlineStr">
-        <is>
-          <t>Total population between age 50-54</t>
-        </is>
-      </c>
+          <t>% Population under 18 years old</t>
+        </is>
+      </c>
+      <c r="V35" t="inlineStr"/>
       <c r="W35" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -3523,12 +3531,12 @@
       </c>
       <c r="X35" t="inlineStr">
         <is>
-          <t>ACS 2018, 5-Year; 2010 Decennial Census; IPUMS NHGIS</t>
+          <t xml:space="preserve">ACS </t>
         </is>
       </c>
       <c r="Y35" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 5 Year Estimates; 2010 Decennial Census; Integrated Public Use Microdata Service National Historic Geographic Information Systems</t>
+          <t>American Community Survey (5-Year Estimate)</t>
         </is>
       </c>
       <c r="AA35" t="inlineStr">
@@ -3538,15 +3546,11 @@
       </c>
       <c r="AB35" t="inlineStr">
         <is>
-          <t>476486</t>
+          <t>60.0</t>
         </is>
       </c>
       <c r="AC35" t="inlineStr"/>
-      <c r="AD35" t="inlineStr">
-        <is>
-          <t>1990 and 2000 data from respective decennial censuses downloaded from IPUMS NHGIS and aggregated upwards.</t>
-        </is>
-      </c>
+      <c r="AD35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3557,44 +3561,40 @@
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
       <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr"/>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
-      <c r="M36" t="inlineStr"/>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr"/>
-      <c r="P36" t="inlineStr"/>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr"/>
       <c r="T36" t="inlineStr">
         <is>
-          <t>AgeOv18</t>
+          <t>Und5P</t>
         </is>
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>Population: Age 18+</t>
-        </is>
-      </c>
-      <c r="V36" t="inlineStr">
-        <is>
-          <t>Total population at or over age 18</t>
-        </is>
-      </c>
+          <t xml:space="preserve">% Population under 5 years old </t>
+        </is>
+      </c>
+      <c r="V36" t="inlineStr"/>
       <c r="W36" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Demographics.md</t>
@@ -3602,12 +3602,12 @@
       </c>
       <c r="X36" t="inlineStr">
         <is>
-          <t>ACS 2018, 5-Year; 2010 Decennial Census</t>
+          <t xml:space="preserve">ACS </t>
         </is>
       </c>
       <c r="Y36" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 5 Year Estimates; 2010 Decennial Census</t>
+          <t>American Community Survey (5-Year Estimate)</t>
         </is>
       </c>
       <c r="AA36" t="inlineStr">
@@ -3617,7 +3617,7 @@
       </c>
       <c r="AB36" t="inlineStr">
         <is>
-          <t>5661461</t>
+          <t>60.0</t>
         </is>
       </c>
       <c r="AC36" t="inlineStr"/>
@@ -5641,8 +5641,16 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr"/>
-      <c r="C65" t="inlineStr"/>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="D65" t="inlineStr">
         <is>
           <t>x</t>
@@ -5664,34 +5672,30 @@
         </is>
       </c>
       <c r="L65" t="inlineStr"/>
-      <c r="M65" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M65" t="inlineStr"/>
       <c r="N65" t="inlineStr"/>
       <c r="O65" t="inlineStr"/>
-      <c r="P65" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P65" t="inlineStr"/>
       <c r="Q65" t="inlineStr"/>
       <c r="R65" t="inlineStr"/>
-      <c r="S65" t="inlineStr"/>
+      <c r="S65" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T65" t="inlineStr">
         <is>
-          <t>DisbP</t>
+          <t>NoHsP</t>
         </is>
       </c>
       <c r="U65" t="inlineStr">
         <is>
-          <t>% Population with Disability</t>
+          <t>% Population without High School Degree</t>
         </is>
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>Percentage of civilian non institutionalized population with a disability</t>
+          <t>Percentage of population 25 years and over, less than a high school degree</t>
         </is>
       </c>
       <c r="W65" t="inlineStr">
@@ -5701,7 +5705,7 @@
       </c>
       <c r="X65" t="inlineStr">
         <is>
-          <t>ACS 2018, 5-Year; ACS 2012, 5-Year</t>
+          <t>ACS 2018, 5-Year; ACS 2012, 5-Year; IPUMS NHGIS</t>
         </is>
       </c>
       <c r="Y65" t="inlineStr">
@@ -5716,15 +5720,15 @@
       </c>
       <c r="AB65" t="inlineStr">
         <is>
-          <t>12.7</t>
-        </is>
-      </c>
-      <c r="AC65" t="inlineStr"/>
-      <c r="AD65" t="inlineStr">
-        <is>
-          <t>Data from 2000 Census downloaded at county level from NHGIS and aggregated upwards.</t>
-        </is>
-      </c>
+          <t>13.01</t>
+        </is>
+      </c>
+      <c r="AC65" t="inlineStr">
+        <is>
+          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
+        </is>
+      </c>
+      <c r="AD65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -5732,16 +5736,8 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr">
         <is>
           <t>x</t>
@@ -5763,30 +5759,34 @@
         </is>
       </c>
       <c r="L66" t="inlineStr"/>
-      <c r="M66" t="inlineStr"/>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N66" t="inlineStr"/>
       <c r="O66" t="inlineStr"/>
-      <c r="P66" t="inlineStr"/>
+      <c r="P66" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q66" t="inlineStr"/>
       <c r="R66" t="inlineStr"/>
-      <c r="S66" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S66" t="inlineStr"/>
       <c r="T66" t="inlineStr">
         <is>
-          <t>NoHsP</t>
+          <t>DisbP</t>
         </is>
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>% Population without High School Degree</t>
+          <t>% Population with Disability</t>
         </is>
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>Percentage of population 25 years and over, less than a high school degree</t>
+          <t>Percentage of civilian non institutionalized population with a disability</t>
         </is>
       </c>
       <c r="W66" t="inlineStr">
@@ -5796,7 +5796,7 @@
       </c>
       <c r="X66" t="inlineStr">
         <is>
-          <t>ACS 2018, 5-Year; ACS 2012, 5-Year; IPUMS NHGIS</t>
+          <t>ACS 2018, 5-Year; ACS 2012, 5-Year</t>
         </is>
       </c>
       <c r="Y66" t="inlineStr">
@@ -5811,15 +5811,15 @@
       </c>
       <c r="AB66" t="inlineStr">
         <is>
-          <t>13.01</t>
-        </is>
-      </c>
-      <c r="AC66" t="inlineStr">
-        <is>
-          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
-        </is>
-      </c>
-      <c r="AD66" t="inlineStr"/>
+          <t>12.7</t>
+        </is>
+      </c>
+      <c r="AC66" t="inlineStr"/>
+      <c r="AD66" t="inlineStr">
+        <is>
+          <t>Data from 2000 Census downloaded at county level from NHGIS and aggregated upwards.</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -5829,15 +5829,15 @@
       </c>
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr"/>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr"/>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="H67" t="inlineStr"/>
       <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr"/>
       <c r="K67" t="inlineStr"/>
@@ -5851,17 +5851,17 @@
       <c r="S67" t="inlineStr"/>
       <c r="T67" t="inlineStr">
         <is>
-          <t>DmySgrg</t>
+          <t>DmyBlckBlt</t>
         </is>
       </c>
       <c r="U67" t="inlineStr">
         <is>
-          <t>Hypersegregated Cities</t>
+          <t>African American South</t>
         </is>
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>Dummy variable for whether county is part of a hypersegregated city or its metropolitan area</t>
+          <t>Dummy variable for whether county is in the Southern Black Belt region</t>
         </is>
       </c>
       <c r="W67" t="inlineStr">
@@ -5871,12 +5871,12 @@
       </c>
       <c r="X67" t="inlineStr">
         <is>
-          <t>Massey et al, 2015</t>
+          <t>US Census, 2000</t>
         </is>
       </c>
       <c r="Y67" t="inlineStr">
         <is>
-          <t>Massey DS, Tannen J. A Research Note on Trends in Black Hypersegregation. Demography. 2015 Jun;52(3):1025-34. doi: 10.1007/s13524-015-0381-6. PMID: 25791615; PMCID: PMC4886656.</t>
+          <t>2000 Decennial Census</t>
         </is>
       </c>
       <c r="AA67" t="inlineStr">
@@ -5886,11 +5886,15 @@
       </c>
       <c r="AB67" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AC67" t="inlineStr"/>
-      <c r="AD67" t="inlineStr"/>
+      <c r="AD67" t="inlineStr">
+        <is>
+          <t>In defining counties in the Southern Black Belt, we included southern US counties where at least 30% of the population identified as Black or African American as of the 2000 Census. However, the Southern Black Belt areas have been variously defined in literature. See, for example, Webster, G. R., &amp; Bowman, J. (2008). Quantitatively Delineating the Black Belt Geographic Region. Southeastern Geographer, 48(1), 3–18. https://doi.org/10.1353/sgo.0.0007.</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -5904,13 +5908,13 @@
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr"/>
-      <c r="H68" t="inlineStr"/>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="I68" t="inlineStr"/>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="J68" t="inlineStr"/>
       <c r="K68" t="inlineStr"/>
       <c r="L68" t="inlineStr"/>
       <c r="M68" t="inlineStr"/>
@@ -5922,17 +5926,17 @@
       <c r="S68" t="inlineStr"/>
       <c r="T68" t="inlineStr">
         <is>
-          <t>PrcNtvRsrv</t>
+          <t>DmySgrg</t>
         </is>
       </c>
       <c r="U68" t="inlineStr">
         <is>
-          <t>Native American &amp; Tribal Lands</t>
+          <t>Hypersegregated Cities</t>
         </is>
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>Percentage of county land area that belongs to Native American reservation(s)</t>
+          <t>Dummy variable for whether county is part of a hypersegregated city or its metropolitan area</t>
         </is>
       </c>
       <c r="W68" t="inlineStr">
@@ -5942,29 +5946,25 @@
       </c>
       <c r="X68" t="inlineStr">
         <is>
-          <t>TIGER/Line 2017</t>
+          <t>Massey et al, 2015</t>
         </is>
       </c>
       <c r="Y68" t="inlineStr">
         <is>
-          <t>TIGER/Line Shapefile, 2017, nation, U.S., Current American Indian/Alaska Native/Native Hawaiian Areas National (AIANNH) National</t>
+          <t>Massey DS, Tannen J. A Research Note on Trends in Black Hypersegregation. Demography. 2015 Jun;52(3):1025-34. doi: 10.1007/s13524-015-0381-6. PMID: 25791615; PMCID: PMC4886656.</t>
         </is>
       </c>
       <c r="AA68" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="AB68" t="inlineStr">
         <is>
-          <t>0.42</t>
-        </is>
-      </c>
-      <c r="AC68" t="inlineStr">
-        <is>
-          <t>The variable representing Native American reservations was calculated as a percent of each county's total land area in US Albers Equal Area projection. Due to consistency issues of spatial projections, there may be some distortion of the percentage of land area calculation in Alaska.</t>
-        </is>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AC68" t="inlineStr"/>
       <c r="AD68" t="inlineStr"/>
     </row>
     <row r="69">
@@ -5975,17 +5975,17 @@
       </c>
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr"/>
-      <c r="J69" t="inlineStr"/>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="K69" t="inlineStr"/>
       <c r="L69" t="inlineStr"/>
       <c r="M69" t="inlineStr"/>
@@ -5997,17 +5997,17 @@
       <c r="S69" t="inlineStr"/>
       <c r="T69" t="inlineStr">
         <is>
-          <t>DmyBlckBlt</t>
+          <t>PrcNtvRsrv</t>
         </is>
       </c>
       <c r="U69" t="inlineStr">
         <is>
-          <t>African American South</t>
+          <t>Native American &amp; Tribal Lands</t>
         </is>
       </c>
       <c r="V69" t="inlineStr">
         <is>
-          <t>Dummy variable for whether county is in the Southern Black Belt region</t>
+          <t>Percentage of county land area that belongs to Native American reservation(s)</t>
         </is>
       </c>
       <c r="W69" t="inlineStr">
@@ -6017,30 +6017,30 @@
       </c>
       <c r="X69" t="inlineStr">
         <is>
-          <t>US Census, 2000</t>
+          <t>TIGER/Line 2017</t>
         </is>
       </c>
       <c r="Y69" t="inlineStr">
         <is>
-          <t>2000 Decennial Census</t>
+          <t>TIGER/Line Shapefile, 2017, nation, U.S., Current American Indian/Alaska Native/Native Hawaiian Areas National (AIANNH) National</t>
         </is>
       </c>
       <c r="AA69" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>number</t>
         </is>
       </c>
       <c r="AB69" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AC69" t="inlineStr"/>
-      <c r="AD69" t="inlineStr">
-        <is>
-          <t>In defining counties in the Southern Black Belt, we included southern US counties where at least 30% of the population identified as Black or African American as of the 2000 Census. However, the Southern Black Belt areas have been variously defined in literature. See, for example, Webster, G. R., &amp; Bowman, J. (2008). Quantitatively Delineating the Black Belt Geographic Region. Southeastern Geographer, 48(1), 3–18. https://doi.org/10.1353/sgo.0.0007.</t>
-        </is>
-      </c>
+          <t>0.42</t>
+        </is>
+      </c>
+      <c r="AC69" t="inlineStr">
+        <is>
+          <t>The variable representing Native American reservations was calculated as a percent of each county's total land area in US Albers Equal Area projection. Due to consistency issues of spatial projections, there may be some distortion of the percentage of land area calculation in Alaska.</t>
+        </is>
+      </c>
+      <c r="AD69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -6285,18 +6285,10 @@
         </is>
       </c>
       <c r="L72" t="inlineStr"/>
-      <c r="M72" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M72" t="inlineStr"/>
       <c r="N72" t="inlineStr"/>
       <c r="O72" t="inlineStr"/>
-      <c r="P72" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P72" t="inlineStr"/>
       <c r="Q72" t="inlineStr"/>
       <c r="R72" t="inlineStr"/>
       <c r="S72" t="inlineStr">
@@ -6306,17 +6298,17 @@
       </c>
       <c r="T72" t="inlineStr">
         <is>
-          <t>AmIndP</t>
+          <t>HispP</t>
         </is>
       </c>
       <c r="U72" t="inlineStr">
         <is>
-          <t>% Native American/Alaska Native Population</t>
+          <t>% Hispanic/Latinx Population</t>
         </is>
       </c>
       <c r="V72" t="inlineStr">
         <is>
-          <t>Percentage of population with race identified as Native American or Alaska Native alone</t>
+          <t>Percentage of population with ethnicity identified as of Hispanic or Latinx origin</t>
         </is>
       </c>
       <c r="W72" t="inlineStr">
@@ -6341,7 +6333,7 @@
       </c>
       <c r="AB72" t="inlineStr">
         <is>
-          <t>0.43</t>
+          <t>25.95</t>
         </is>
       </c>
       <c r="AC72" t="inlineStr">
@@ -6409,17 +6401,17 @@
       </c>
       <c r="T73" t="inlineStr">
         <is>
-          <t>PacIsP</t>
+          <t>AmIndP</t>
         </is>
       </c>
       <c r="U73" t="inlineStr">
         <is>
-          <t>% Native Hawaiian &amp; Other PI Population</t>
+          <t>% Native American/Alaska Native Population</t>
         </is>
       </c>
       <c r="V73" t="inlineStr">
         <is>
-          <t>Percentage of population with race identified as Native Hawaiian and Other Pacific Islander alone</t>
+          <t>Percentage of population with race identified as Native American or Alaska Native alone</t>
         </is>
       </c>
       <c r="W73" t="inlineStr">
@@ -6444,7 +6436,7 @@
       </c>
       <c r="AB73" t="inlineStr">
         <is>
-          <t>0.05</t>
+          <t>0.43</t>
         </is>
       </c>
       <c r="AC73" t="inlineStr">
@@ -6491,18 +6483,10 @@
         </is>
       </c>
       <c r="L74" t="inlineStr"/>
-      <c r="M74" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M74" t="inlineStr"/>
       <c r="N74" t="inlineStr"/>
       <c r="O74" t="inlineStr"/>
-      <c r="P74" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P74" t="inlineStr"/>
       <c r="Q74" t="inlineStr"/>
       <c r="R74" t="inlineStr"/>
       <c r="S74" t="inlineStr">
@@ -6512,17 +6496,17 @@
       </c>
       <c r="T74" t="inlineStr">
         <is>
-          <t>OtherP</t>
+          <t>AsianP</t>
         </is>
       </c>
       <c r="U74" t="inlineStr">
         <is>
-          <t>% Other (race) Population</t>
+          <t>% Asian Population</t>
         </is>
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>Percentage of Population with race not mentioned in any of the options above (includes two race or more races)</t>
+          <t>Percentage of population with race identified as Asian alone</t>
         </is>
       </c>
       <c r="W74" t="inlineStr">
@@ -6547,7 +6531,7 @@
       </c>
       <c r="AB74" t="inlineStr">
         <is>
-          <t>16.48</t>
+          <t>12.03</t>
         </is>
       </c>
       <c r="AC74" t="inlineStr">
@@ -6563,16 +6547,36 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr"/>
-      <c r="C75" t="inlineStr"/>
-      <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr"/>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
       <c r="I75" t="inlineStr"/>
       <c r="J75" t="inlineStr"/>
-      <c r="K75" t="inlineStr"/>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L75" t="inlineStr"/>
       <c r="M75" t="inlineStr">
         <is>
@@ -6588,18 +6592,26 @@
       </c>
       <c r="Q75" t="inlineStr"/>
       <c r="R75" t="inlineStr"/>
-      <c r="S75" t="inlineStr"/>
+      <c r="S75" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T75" t="inlineStr">
         <is>
-          <t>HisP</t>
+          <t>PacIsP</t>
         </is>
       </c>
       <c r="U75" t="inlineStr">
         <is>
-          <t>% Population with ethnicity identified as of Hispanic or Latinx origin</t>
-        </is>
-      </c>
-      <c r="V75" t="inlineStr"/>
+          <t>% Native Hawaiian &amp; Other PI Population</t>
+        </is>
+      </c>
+      <c r="V75" t="inlineStr">
+        <is>
+          <t>Percentage of population with race identified as Native Hawaiian and Other Pacific Islander alone</t>
+        </is>
+      </c>
       <c r="W75" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Race_Ethnicity.md</t>
@@ -6607,12 +6619,12 @@
       </c>
       <c r="X75" t="inlineStr">
         <is>
-          <t xml:space="preserve">ACS </t>
+          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
         </is>
       </c>
       <c r="Y75" t="inlineStr">
         <is>
-          <t>American Community Survey (5-Year Estimate)</t>
+          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
         </is>
       </c>
       <c r="AA75" t="inlineStr">
@@ -6622,10 +6634,14 @@
       </c>
       <c r="AB75" t="inlineStr">
         <is>
-          <t>60.0</t>
-        </is>
-      </c>
-      <c r="AC75" t="inlineStr"/>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="AC75" t="inlineStr">
+        <is>
+          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
+        </is>
+      </c>
       <c r="AD75" t="inlineStr"/>
     </row>
     <row r="76">
@@ -6634,16 +6650,36 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr"/>
-      <c r="C76" t="inlineStr"/>
-      <c r="D76" t="inlineStr"/>
-      <c r="E76" t="inlineStr"/>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
       <c r="I76" t="inlineStr"/>
       <c r="J76" t="inlineStr"/>
-      <c r="K76" t="inlineStr"/>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L76" t="inlineStr"/>
       <c r="M76" t="inlineStr">
         <is>
@@ -6659,18 +6695,26 @@
       </c>
       <c r="Q76" t="inlineStr"/>
       <c r="R76" t="inlineStr"/>
-      <c r="S76" t="inlineStr"/>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T76" t="inlineStr">
         <is>
-          <t>TwoRaceP</t>
+          <t>OtherP</t>
         </is>
       </c>
       <c r="U76" t="inlineStr">
         <is>
-          <t>% Population identifying as two or more races</t>
-        </is>
-      </c>
-      <c r="V76" t="inlineStr"/>
+          <t>% Other (race) Population</t>
+        </is>
+      </c>
+      <c r="V76" t="inlineStr">
+        <is>
+          <t>Percentage of Population with race not mentioned in any of the options above (includes two race or more races)</t>
+        </is>
+      </c>
       <c r="W76" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Race_Ethnicity.md</t>
@@ -6678,12 +6722,12 @@
       </c>
       <c r="X76" t="inlineStr">
         <is>
-          <t xml:space="preserve">ACS </t>
+          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
         </is>
       </c>
       <c r="Y76" t="inlineStr">
         <is>
-          <t>American Community Survey (5-Year Estimate)</t>
+          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
         </is>
       </c>
       <c r="AA76" t="inlineStr">
@@ -6693,10 +6737,14 @@
       </c>
       <c r="AB76" t="inlineStr">
         <is>
-          <t>60.0</t>
-        </is>
-      </c>
-      <c r="AC76" t="inlineStr"/>
+          <t>16.48</t>
+        </is>
+      </c>
+      <c r="AC76" t="inlineStr">
+        <is>
+          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
+        </is>
+      </c>
       <c r="AD76" t="inlineStr"/>
     </row>
     <row r="77">
@@ -6705,63 +6753,43 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr"/>
+      <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr"/>
       <c r="I77" t="inlineStr"/>
       <c r="J77" t="inlineStr"/>
-      <c r="K77" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K77" t="inlineStr"/>
       <c r="L77" t="inlineStr"/>
-      <c r="M77" t="inlineStr"/>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N77" t="inlineStr"/>
       <c r="O77" t="inlineStr"/>
-      <c r="P77" t="inlineStr"/>
+      <c r="P77" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q77" t="inlineStr"/>
       <c r="R77" t="inlineStr"/>
-      <c r="S77" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S77" t="inlineStr"/>
       <c r="T77" t="inlineStr">
         <is>
-          <t>HispP</t>
+          <t>HisP</t>
         </is>
       </c>
       <c r="U77" t="inlineStr">
         <is>
-          <t>% Hispanic/Latinx Population</t>
-        </is>
-      </c>
-      <c r="V77" t="inlineStr">
-        <is>
-          <t>Percentage of population with ethnicity identified as of Hispanic or Latinx origin</t>
-        </is>
-      </c>
+          <t>% Population with ethnicity identified as of Hispanic or Latinx origin</t>
+        </is>
+      </c>
+      <c r="V77" t="inlineStr"/>
       <c r="W77" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Race_Ethnicity.md</t>
@@ -6769,12 +6797,12 @@
       </c>
       <c r="X77" t="inlineStr">
         <is>
-          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
+          <t xml:space="preserve">ACS </t>
         </is>
       </c>
       <c r="Y77" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
+          <t>American Community Survey (5-Year Estimate)</t>
         </is>
       </c>
       <c r="AA77" t="inlineStr">
@@ -6784,14 +6812,10 @@
       </c>
       <c r="AB77" t="inlineStr">
         <is>
-          <t>25.95</t>
-        </is>
-      </c>
-      <c r="AC77" t="inlineStr">
-        <is>
-          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
-        </is>
-      </c>
+          <t>60.0</t>
+        </is>
+      </c>
+      <c r="AC77" t="inlineStr"/>
       <c r="AD77" t="inlineStr"/>
     </row>
     <row r="78">
@@ -6800,63 +6824,43 @@
           <t>Social</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr"/>
+      <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="inlineStr"/>
       <c r="I78" t="inlineStr"/>
       <c r="J78" t="inlineStr"/>
-      <c r="K78" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K78" t="inlineStr"/>
       <c r="L78" t="inlineStr"/>
-      <c r="M78" t="inlineStr"/>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N78" t="inlineStr"/>
       <c r="O78" t="inlineStr"/>
-      <c r="P78" t="inlineStr"/>
+      <c r="P78" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q78" t="inlineStr"/>
       <c r="R78" t="inlineStr"/>
-      <c r="S78" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S78" t="inlineStr"/>
       <c r="T78" t="inlineStr">
         <is>
-          <t>AsianP</t>
+          <t>TwoRaceP</t>
         </is>
       </c>
       <c r="U78" t="inlineStr">
         <is>
-          <t>% Asian Population</t>
-        </is>
-      </c>
-      <c r="V78" t="inlineStr">
-        <is>
-          <t>Percentage of population with race identified as Asian alone</t>
-        </is>
-      </c>
+          <t>% Population identifying as two or more races</t>
+        </is>
+      </c>
+      <c r="V78" t="inlineStr"/>
       <c r="W78" t="inlineStr">
         <is>
           <t>https://github.com/GeoDaCenter/opioid-policy-scan/blob/main/data_final/metadata/Race_Ethnicity.md</t>
@@ -6864,12 +6868,12 @@
       </c>
       <c r="X78" t="inlineStr">
         <is>
-          <t>ACS 2018, 5-Year; Census 2010; IPUMS NHGIS</t>
+          <t xml:space="preserve">ACS </t>
         </is>
       </c>
       <c r="Y78" t="inlineStr">
         <is>
-          <t>American Community Survey 2014-2018 5 Year Estimate; 2010 Decennial Census; Integrated Public Use Microdata Series National Historic Geographic Information System</t>
+          <t>American Community Survey (5-Year Estimate)</t>
         </is>
       </c>
       <c r="AA78" t="inlineStr">
@@ -6879,14 +6883,10 @@
       </c>
       <c r="AB78" t="inlineStr">
         <is>
-          <t>12.03</t>
-        </is>
-      </c>
-      <c r="AC78" t="inlineStr">
-        <is>
-          <t>1980-2000 historic data was acquired from NHGIS and then interpolated to modern county boundaries through a population weighted interpolation using the tidycensus `interpolate_pw` function. For 1980, the underlying population weighting was county subdivisions, while for 1990 and 200 the underlying population weighting was tracts.</t>
-        </is>
-      </c>
+          <t>60.0</t>
+        </is>
+      </c>
+      <c r="AC78" t="inlineStr"/>
       <c r="AD78" t="inlineStr"/>
     </row>
     <row r="79">
@@ -8694,7 +8694,7 @@
       <c r="S101" t="inlineStr"/>
       <c r="T101" t="inlineStr">
         <is>
-          <t>NalCtTmDr</t>
+          <t>NaltCtTmDr</t>
         </is>
       </c>
       <c r="U101" t="inlineStr">
@@ -8777,7 +8777,7 @@
       <c r="S102" t="inlineStr"/>
       <c r="T102" t="inlineStr">
         <is>
-          <t>NalCtTmBk</t>
+          <t>NaltCtTmBk</t>
         </is>
       </c>
       <c r="U102" t="inlineStr">
@@ -8860,7 +8860,7 @@
       <c r="S103" t="inlineStr"/>
       <c r="T103" t="inlineStr">
         <is>
-          <t>NalCtTmWk</t>
+          <t>NaltCtTmWk</t>
         </is>
       </c>
       <c r="U103" t="inlineStr">
@@ -9441,7 +9441,7 @@
       <c r="S110" t="inlineStr"/>
       <c r="T110" t="inlineStr">
         <is>
-          <t>NalAvTmDr</t>
+          <t>NaltAvTmDr</t>
         </is>
       </c>
       <c r="U110" t="inlineStr">
@@ -9524,7 +9524,7 @@
       <c r="S111" t="inlineStr"/>
       <c r="T111" t="inlineStr">
         <is>
-          <t>NalAvTmBk</t>
+          <t>NaltAvTmBk</t>
         </is>
       </c>
       <c r="U111" t="inlineStr">
@@ -9607,7 +9607,7 @@
       <c r="S112" t="inlineStr"/>
       <c r="T112" t="inlineStr">
         <is>
-          <t>NalAvTmWk</t>
+          <t>NaltAvTmWk</t>
         </is>
       </c>
       <c r="U112" t="inlineStr">
@@ -10188,7 +10188,7 @@
       <c r="S119" t="inlineStr"/>
       <c r="T119" t="inlineStr">
         <is>
-          <t>NalTmDrP</t>
+          <t>NaltTmDrP</t>
         </is>
       </c>
       <c r="U119" t="inlineStr">
@@ -10271,7 +10271,7 @@
       <c r="S120" t="inlineStr"/>
       <c r="T120" t="inlineStr">
         <is>
-          <t>NalTmBkP</t>
+          <t>NaltTmBkP</t>
         </is>
       </c>
       <c r="U120" t="inlineStr">
@@ -10354,7 +10354,7 @@
       <c r="S121" t="inlineStr"/>
       <c r="T121" t="inlineStr">
         <is>
-          <t>NalTmWkP</t>
+          <t>NaltTmWkP</t>
         </is>
       </c>
       <c r="U121" t="inlineStr">
@@ -12809,17 +12809,17 @@
       <c r="B152" t="inlineStr"/>
       <c r="C152" t="inlineStr"/>
       <c r="D152" t="inlineStr"/>
-      <c r="E152" t="inlineStr"/>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="F152" t="inlineStr"/>
       <c r="G152" t="inlineStr"/>
       <c r="H152" t="inlineStr"/>
       <c r="I152" t="inlineStr"/>
       <c r="J152" t="inlineStr"/>
-      <c r="K152" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K152" t="inlineStr"/>
       <c r="L152" t="inlineStr"/>
       <c r="M152" t="inlineStr"/>
       <c r="N152" t="inlineStr"/>
@@ -12830,17 +12830,17 @@
       <c r="S152" t="inlineStr"/>
       <c r="T152" t="inlineStr">
         <is>
-          <t>RcaUrbanP</t>
+          <t>RuralPop</t>
         </is>
       </c>
       <c r="U152" t="inlineStr">
         <is>
-          <t>% Tracts Urban (RUCA)</t>
+          <t>Rural Population</t>
         </is>
       </c>
       <c r="V152" t="inlineStr">
         <is>
-          <t>Percent census tracts in the county classified as Urban using RUCA codes</t>
+          <t>2010 Population living in non urban areas, as defined by Census Bureau</t>
         </is>
       </c>
       <c r="W152" t="inlineStr">
@@ -12860,12 +12860,12 @@
       </c>
       <c r="AA152" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="AB152" t="inlineStr">
         <is>
-          <t>0.99</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AC152" t="inlineStr"/>
@@ -12905,17 +12905,17 @@
       <c r="S153" t="inlineStr"/>
       <c r="T153" t="inlineStr">
         <is>
-          <t>RcaSubrbP</t>
+          <t>RcaUrbanP</t>
         </is>
       </c>
       <c r="U153" t="inlineStr">
         <is>
-          <t>% Tracts Suburban (RUCA)</t>
+          <t>% Tracts Urban (RUCA)</t>
         </is>
       </c>
       <c r="V153" t="inlineStr">
         <is>
-          <t>Percent census tracts in the county classified as Suburban using RUCA codes</t>
+          <t>Percent census tracts in the county classified as Urban using RUCA codes</t>
         </is>
       </c>
       <c r="W153" t="inlineStr">
@@ -12940,7 +12940,7 @@
       </c>
       <c r="AB153" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.99</t>
         </is>
       </c>
       <c r="AC153" t="inlineStr"/>
@@ -12980,17 +12980,17 @@
       <c r="S154" t="inlineStr"/>
       <c r="T154" t="inlineStr">
         <is>
-          <t>RcaRuralP</t>
+          <t>RcaSubrbP</t>
         </is>
       </c>
       <c r="U154" t="inlineStr">
         <is>
-          <t>% Tracts Rural (RUCA)</t>
+          <t>% Tracts Suburban (RUCA)</t>
         </is>
       </c>
       <c r="V154" t="inlineStr">
         <is>
-          <t>Percent census tracts in the county classified as Rural using RUCA codes</t>
+          <t>Percent census tracts in the county classified as Suburban using RUCA codes</t>
         </is>
       </c>
       <c r="W154" t="inlineStr">
@@ -13015,7 +13015,7 @@
       </c>
       <c r="AB154" t="inlineStr">
         <is>
-          <t>0.01</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AC154" t="inlineStr"/>
@@ -13055,17 +13055,17 @@
       <c r="S155" t="inlineStr"/>
       <c r="T155" t="inlineStr">
         <is>
-          <t>CenRuralP</t>
+          <t>RcaRuralP</t>
         </is>
       </c>
       <c r="U155" t="inlineStr">
         <is>
-          <t>Rural Population % (2010)</t>
+          <t>% Tracts Rural (RUCA)</t>
         </is>
       </c>
       <c r="V155" t="inlineStr">
         <is>
-          <t>% of 2010 Population living in non urban areas, as defined by Census Bureau</t>
+          <t>Percent census tracts in the county classified as Rural using RUCA codes</t>
         </is>
       </c>
       <c r="W155" t="inlineStr">
@@ -13090,7 +13090,7 @@
       </c>
       <c r="AB155" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.01</t>
         </is>
       </c>
       <c r="AC155" t="inlineStr"/>
@@ -13109,17 +13109,17 @@
       <c r="B156" t="inlineStr"/>
       <c r="C156" t="inlineStr"/>
       <c r="D156" t="inlineStr"/>
-      <c r="E156" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="E156" t="inlineStr"/>
       <c r="F156" t="inlineStr"/>
       <c r="G156" t="inlineStr"/>
       <c r="H156" t="inlineStr"/>
       <c r="I156" t="inlineStr"/>
       <c r="J156" t="inlineStr"/>
-      <c r="K156" t="inlineStr"/>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L156" t="inlineStr"/>
       <c r="M156" t="inlineStr"/>
       <c r="N156" t="inlineStr"/>
@@ -13130,17 +13130,17 @@
       <c r="S156" t="inlineStr"/>
       <c r="T156" t="inlineStr">
         <is>
-          <t>RuralPop</t>
+          <t>CenRuralP</t>
         </is>
       </c>
       <c r="U156" t="inlineStr">
         <is>
-          <t>Rural Population</t>
+          <t>Rural Population % (2010)</t>
         </is>
       </c>
       <c r="V156" t="inlineStr">
         <is>
-          <t>2010 Population living in non urban areas, as defined by Census Bureau</t>
+          <t>% of 2010 Population living in non urban areas, as defined by Census Bureau</t>
         </is>
       </c>
       <c r="W156" t="inlineStr">
@@ -13160,7 +13160,7 @@
       </c>
       <c r="AA156" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>number</t>
         </is>
       </c>
       <c r="AB156" t="inlineStr">
@@ -14228,34 +14228,26 @@
         </is>
       </c>
       <c r="L169" t="inlineStr"/>
-      <c r="M169" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M169" t="inlineStr"/>
       <c r="N169" t="inlineStr"/>
       <c r="O169" t="inlineStr"/>
-      <c r="P169" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P169" t="inlineStr"/>
       <c r="Q169" t="inlineStr"/>
       <c r="R169" t="inlineStr"/>
       <c r="S169" t="inlineStr"/>
       <c r="T169" t="inlineStr">
         <is>
-          <t>EssnWrkP</t>
+          <t>EssnWrkE</t>
         </is>
       </c>
       <c r="U169" t="inlineStr">
         <is>
-          <t>Essential Workers %</t>
+          <t>Count of Essential Workers</t>
         </is>
       </c>
       <c r="V169" t="inlineStr">
         <is>
-          <t>Percentage of population employed in essential occupations.</t>
+          <t>Estimated count of population employed in essential occupations.</t>
         </is>
       </c>
       <c r="W169" t="inlineStr">
@@ -14275,12 +14267,12 @@
       </c>
       <c r="AA169" t="inlineStr">
         <is>
-          <t>number</t>
+          <t>integer</t>
         </is>
       </c>
       <c r="AB169" t="inlineStr">
         <is>
-          <t>42.96</t>
+          <t>1509709</t>
         </is>
       </c>
       <c r="AC169" t="inlineStr"/>
@@ -14307,26 +14299,34 @@
         </is>
       </c>
       <c r="L170" t="inlineStr"/>
-      <c r="M170" t="inlineStr"/>
+      <c r="M170" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N170" t="inlineStr"/>
       <c r="O170" t="inlineStr"/>
-      <c r="P170" t="inlineStr"/>
+      <c r="P170" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q170" t="inlineStr"/>
       <c r="R170" t="inlineStr"/>
       <c r="S170" t="inlineStr"/>
       <c r="T170" t="inlineStr">
         <is>
-          <t>EssnWrkE</t>
+          <t>EssnWrkP</t>
         </is>
       </c>
       <c r="U170" t="inlineStr">
         <is>
-          <t>Count of Essential Workers</t>
+          <t>Essential Workers %</t>
         </is>
       </c>
       <c r="V170" t="inlineStr">
         <is>
-          <t>Estimated count of population employed in essential occupations.</t>
+          <t>Percentage of population employed in essential occupations.</t>
         </is>
       </c>
       <c r="W170" t="inlineStr">
@@ -14346,12 +14346,12 @@
       </c>
       <c r="AA170" t="inlineStr">
         <is>
-          <t>integer</t>
+          <t>number</t>
         </is>
       </c>
       <c r="AB170" t="inlineStr">
         <is>
-          <t>1509709</t>
+          <t>42.96</t>
         </is>
       </c>
       <c r="AC170" t="inlineStr"/>
@@ -15158,18 +15158,46 @@
       <c r="D181" t="inlineStr"/>
       <c r="E181" t="inlineStr"/>
       <c r="F181" t="inlineStr"/>
-      <c r="G181" t="inlineStr"/>
-      <c r="H181" t="inlineStr"/>
-      <c r="I181" t="inlineStr"/>
-      <c r="J181" t="inlineStr"/>
-      <c r="K181" t="inlineStr"/>
-      <c r="L181" t="inlineStr"/>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I181" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="J181" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="L181" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M181" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="N181" t="inlineStr"/>
+      <c r="N181" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O181" t="inlineStr">
         <is>
           <t>x</t>
@@ -15181,17 +15209,17 @@
       <c r="S181" t="inlineStr"/>
       <c r="T181" t="inlineStr">
         <is>
-          <t>OpRxRt</t>
+          <t>OdMortRt</t>
         </is>
       </c>
       <c r="U181" t="inlineStr">
         <is>
-          <t>Opioid Prescription Rate</t>
+          <t>Overdose Mortality Rate</t>
         </is>
       </c>
       <c r="V181" t="inlineStr">
         <is>
-          <t>Opioid prescription rate</t>
+          <t>Overdose mortality rate</t>
         </is>
       </c>
       <c r="W181" t="inlineStr">
@@ -15216,7 +15244,7 @@
       </c>
       <c r="AB181" t="inlineStr">
         <is>
-          <t>39.5</t>
+          <t>13.3</t>
         </is>
       </c>
       <c r="AC181" t="inlineStr"/>
@@ -15233,46 +15261,18 @@
       <c r="D182" t="inlineStr"/>
       <c r="E182" t="inlineStr"/>
       <c r="F182" t="inlineStr"/>
-      <c r="G182" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="H182" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="I182" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="J182" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="K182" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="L182" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="G182" t="inlineStr"/>
+      <c r="H182" t="inlineStr"/>
+      <c r="I182" t="inlineStr"/>
+      <c r="J182" t="inlineStr"/>
+      <c r="K182" t="inlineStr"/>
+      <c r="L182" t="inlineStr"/>
       <c r="M182" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="N182" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N182" t="inlineStr"/>
       <c r="O182" t="inlineStr">
         <is>
           <t>x</t>
@@ -15284,17 +15284,17 @@
       <c r="S182" t="inlineStr"/>
       <c r="T182" t="inlineStr">
         <is>
-          <t>OdMortRt</t>
+          <t>OpRxRt</t>
         </is>
       </c>
       <c r="U182" t="inlineStr">
         <is>
-          <t>Overdose Mortality Rate</t>
+          <t>Opioid Prescription Rate</t>
         </is>
       </c>
       <c r="V182" t="inlineStr">
         <is>
-          <t>Overdose mortality rate</t>
+          <t>Opioid prescription rate</t>
         </is>
       </c>
       <c r="W182" t="inlineStr">
@@ -15319,7 +15319,7 @@
       </c>
       <c r="AB182" t="inlineStr">
         <is>
-          <t>13.3</t>
+          <t>39.5</t>
         </is>
       </c>
       <c r="AC182" t="inlineStr"/>

</xml_diff>

<commit_message>
updated data dictionaries #121
</commit_message>
<xml_diff>
--- a/backend/oeps/data/dictionaries/C_Dict.xlsx
+++ b/backend/oeps/data/dictionaries/C_Dict.xlsx
@@ -982,17 +982,17 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>GEOID</t>
+          <t>FIPS</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>GEOID</t>
+          <t>Federal Information Processing Standard code</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>Unique identifer for the geography unit to which this value should be attached</t>
+          <t>Federal Information Processing Standard code designated by the NIST; is two digits for states, five digits for counties, eleven digits for tracts.</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">

</xml_diff>